<commit_message>
fix: update S3 path to HotelLeadGen/{country}/{state}/{file}.xlsx
</commit_message>
<xml_diff>
--- a/Miami_Beach.xlsx
+++ b/Miami_Beach.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,9 +453,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="60" customWidth="1" min="1" max="1"/>
-    <col width="28" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="41" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="2" max="2"/>
+    <col width="28" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="41" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -466,15 +467,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Website</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Booking Engine</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Room Count</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Proximity</t>
         </is>
@@ -488,13 +494,18 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
+          <t>http://www.aquamiami.com/?utm_source=gmb&amp;utm_medium=organic</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="D2" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.3km)</t>
         </is>
@@ -508,13 +519,18 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
+          <t>http://thebetsyhotel.com/</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
           <t>Triptease</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="D3" s="2" t="n">
         <v>1564</v>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -528,13 +544,18 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
+          <t>https://stayviax.com/hotel/72296725</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="D4" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.9km)</t>
         </is>
@@ -548,13 +569,18 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
+          <t>https://www.boulanmiami.com/</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="D5" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.2km)</t>
         </is>
@@ -568,13 +594,18 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
+          <t>https://boutiqueapartmentsmiami.hostify.club/</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="D6" s="2" t="n">
         <v>600</v>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.2km)</t>
         </is>
@@ -588,13 +619,18 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
+          <t>https://cardozohotel.com/?utm_source=google&amp;utm_medium=organic&amp;utm_campaign=mybusiness</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="D7" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.2km)</t>
         </is>
@@ -608,13 +644,18 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
+          <t>https://www.oasiscasitacollection.com/resorts/miami-beach/oasis/casa-gaby-apartments/</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
           <t>WebRez</t>
         </is>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.0km)</t>
         </is>
@@ -628,13 +669,18 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
+          <t>https://casahotelsgroup.com/casa-sobe/</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
           <t>Cloudbeds</t>
         </is>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="D9" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.2km)</t>
         </is>
@@ -648,13 +694,18 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
+          <t>https://www.casahotelsgroup.com/casa-sofi</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
           <t>Cloudbeds</t>
         </is>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="D10" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.7km)</t>
         </is>
@@ -668,13 +719,18 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
+          <t>https://www.circa39.com/?utm_medium=organic&amp;utm_source=google&amp;utm_campaign=business-listing</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="D11" s="2" t="n">
         <v>97</v>
       </c>
-      <c r="D11" s="2" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (3.0km)</t>
         </is>
@@ -688,13 +744,18 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
+          <t>https://www.clevelander.com/</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="D12" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.6km)</t>
         </is>
@@ -708,13 +769,18 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
+          <t>https://www.oasiscasitacollection.com/resorts/miami-beach/oasis/courtyard-apartments/</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
           <t>WebRez</t>
         </is>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="D13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="inlineStr">
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.8km)</t>
         </is>
@@ -728,13 +794,18 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
+          <t>https://alexanderhotel.holidayfuture.com/listings/377669?googleVR=1&amp;utm_source=google&amp;utm_medium=vacation_rentals</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="D14" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D14" s="2" t="inlineStr">
+      <c r="E14" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (2.1km)</t>
         </is>
@@ -748,13 +819,18 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
+          <t>https://www.esmehotel.com/?utm_source=local-listings&amp;utm_medium=organic&amp;utm_campaign=local-listings</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="D15" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D15" s="2" t="inlineStr">
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.2km)</t>
         </is>
@@ -768,13 +844,18 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
+          <t>https://www.essexhotel.com/</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="D16" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="2" t="inlineStr">
+      <c r="E16" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.6km)</t>
         </is>
@@ -788,13 +869,18 @@
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
+          <t>https://fontainebleau.com/?utm_source=google-local&amp;utm_medium=organic&amp;utm_campaign=gmb</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="D17" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D17" s="2" t="inlineStr">
+      <c r="E17" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (3.5km)</t>
         </is>
@@ -808,13 +894,18 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
+          <t>https://franklinsuitessouthbeach.com/</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
           <t>Guesty</t>
         </is>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="D18" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D18" s="2" t="inlineStr">
+      <c r="E18" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.8km)</t>
         </is>
@@ -828,13 +919,18 @@
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
+          <t>https://staygenerator.com/hotels/miami?utm_source=google-my-business&amp;utm_medium=organic&amp;utm_campaign=hostel-Miami</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
           <t>Mews</t>
         </is>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="D19" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D19" s="2" t="inlineStr">
+      <c r="E19" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (2.4km)</t>
         </is>
@@ -848,13 +944,18 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
+          <t>https://www.globalluxurysuites.com/property/78111/fl/miami-beach/global-luxury-suites-at-the-apex-miami</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="D20" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="inlineStr">
+      <c r="E20" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.4km)</t>
         </is>
@@ -868,13 +969,18 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
+          <t>https://lowkl.com/property/greenview-by-lowkl/</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
           <t>Cloudbeds</t>
         </is>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="D21" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="2" t="inlineStr">
+      <c r="E21" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.7km)</t>
         </is>
@@ -888,13 +994,18 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
+          <t>https://www.bellezahotel.com/</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
           <t>WebRez</t>
         </is>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="D22" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="D22" s="2" t="inlineStr">
+      <c r="E22" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.3km)</t>
         </is>
@@ -908,13 +1019,18 @@
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
+          <t>https://thehotelchelsea.com/</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="D23" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D23" s="2" t="inlineStr">
+      <c r="E23" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.7km)</t>
         </is>
@@ -928,13 +1044,18 @@
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
+          <t>https://hotelcroydonmiamibeach.com/</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="D24" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D24" s="2" t="inlineStr">
+      <c r="E24" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (2.8km)</t>
         </is>
@@ -948,13 +1069,18 @@
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
+          <t>https://www.greystonehotel.com/?utm_source=google&amp;utm_medium=organic&amp;utm_campaign=business_listing</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C25" s="2" t="n">
+      <c r="D25" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D25" s="2" t="inlineStr">
+      <c r="E25" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.1km)</t>
         </is>
@@ -968,13 +1094,18 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
+          <t>https://islandhousesouthbeach.com/</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C26" s="2" t="n">
+      <c r="D26" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="2" t="inlineStr">
+      <c r="E26" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -988,13 +1119,18 @@
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
+          <t>https://www.islandsofmiami.com/</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n">
+      <c r="D27" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D27" s="2" t="inlineStr">
+      <c r="E27" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (3.0km)</t>
         </is>
@@ -1008,13 +1144,18 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
+          <t>https://kasa.com/properties/kasa-collins-park-miami-beach-convention-center?utm_source=Google&amp;utm_medium=nonpaid&amp;utm_campaign=GMB&amp;utm_term=VisitHotelWebsiteButton&amp;utm_content=CPK</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
           <t>Triptease</t>
         </is>
       </c>
-      <c r="C28" s="2" t="n">
+      <c r="D28" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D28" s="2" t="inlineStr">
+      <c r="E28" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.4km)</t>
         </is>
@@ -1028,13 +1169,18 @@
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
+          <t>https://kasa.com/properties/kasa-el-paseo-miami-beach?utm_source=Google&amp;utm_medium=nonpaid&amp;utm_campaign=GMB&amp;utm_term=VisitHotelWebsiteButton&amp;utm_content=PAS</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
           <t>Triptease</t>
         </is>
       </c>
-      <c r="C29" s="2" t="n">
+      <c r="D29" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="2" t="inlineStr">
+      <c r="E29" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.3km)</t>
         </is>
@@ -1048,13 +1194,18 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
+          <t>https://thekaskadeshotel.com/</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
           <t>Clock PMS</t>
         </is>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="D30" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D30" s="2" t="inlineStr">
+      <c r="E30" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.7km)</t>
         </is>
@@ -1068,13 +1219,18 @@
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
+          <t>https://www.kenmorevillagehotel.com/</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C31" s="2" t="n">
+      <c r="D31" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D31" s="2" t="inlineStr">
+      <c r="E31" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.6km)</t>
         </is>
@@ -1088,13 +1244,18 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
+          <t>https://www.surfcomber.com/?&amp;cm_mmc=WEB-_-KI-_-AMER-_-EN-_-EV-_-Google%20Business%20Profile-_-DD-_-surfcomber</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
           <t>IHG</t>
         </is>
       </c>
-      <c r="C32" s="2" t="n">
+      <c r="D32" s="2" t="n">
         <v>186</v>
       </c>
-      <c r="D32" s="2" t="inlineStr">
+      <c r="E32" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.8km)</t>
         </is>
@@ -1108,13 +1269,18 @@
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
+          <t>https://www.leparticuliermiami.com/</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C33" s="2" t="n">
+      <c r="D33" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D33" s="2" t="inlineStr">
+      <c r="E33" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (3.2km)</t>
         </is>
@@ -1128,13 +1294,18 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
+          <t>https://lesliehotel.com/</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
           <t>IQWebBook</t>
         </is>
       </c>
-      <c r="C34" s="2" t="n">
+      <c r="D34" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="D34" s="2" t="inlineStr">
+      <c r="E34" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.3km)</t>
         </is>
@@ -1148,13 +1319,18 @@
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
+          <t>https://www.deco305.com/</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C35" s="2" t="n">
+      <c r="D35" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="D35" s="2" t="inlineStr">
+      <c r="E35" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.2km)</t>
         </is>
@@ -1168,13 +1344,18 @@
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
+          <t>https://luxuri.com/?utm_campaign=gmb</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C36" s="2" t="n">
+      <c r="D36" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D36" s="2" t="inlineStr">
+      <c r="E36" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.0km)</t>
         </is>
@@ -1188,13 +1369,18 @@
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
+          <t>http://www.luxurisuites.com/</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C37" s="2" t="n">
+      <c r="D37" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D37" s="2" t="inlineStr">
+      <c r="E37" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.8km)</t>
         </is>
@@ -1208,13 +1394,18 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
+          <t>https://alexanderhotel.holidayfuture.com/listings/274633?googleVR=1&amp;utm_source=google&amp;utm_medium=vacation_rentals</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C38" s="2" t="n">
+      <c r="D38" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D38" s="2" t="inlineStr">
+      <c r="E38" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (2.1km)</t>
         </is>
@@ -1228,13 +1419,18 @@
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
+          <t>https://www.luxuryrentalsmiamibeach.com/?utm_source=google&amp;utm_medium=organic&amp;utm_campaign=gbp</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="inlineStr">
+        <is>
           <t>Track</t>
         </is>
       </c>
-      <c r="C39" s="2" t="n">
+      <c r="D39" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D39" s="2" t="inlineStr">
+      <c r="E39" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (3.1km)</t>
         </is>
@@ -1248,13 +1444,18 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
+          <t>https://mdqwatersports.com/</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="inlineStr">
+        <is>
           <t>FareHarbor</t>
         </is>
       </c>
-      <c r="C40" s="2" t="n">
+      <c r="D40" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D40" s="2" t="inlineStr">
+      <c r="E40" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (2.1km)</t>
         </is>
@@ -1268,13 +1469,18 @@
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
+          <t>https://www.vacasa.com/usa/Florida/Miami-Beach/?utm_source=gmb&amp;utm_medium=organic&amp;utm_campaign=GMB-Miami-Vacation-Rentals</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C41" s="2" t="n">
+      <c r="D41" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D41" s="2" t="inlineStr">
+      <c r="E41" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (1.7km)</t>
         </is>
@@ -1288,13 +1494,18 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
+          <t>https://lowkl.com/property/miami-beach-international/</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
           <t>Cloudbeds</t>
         </is>
       </c>
-      <c r="C42" s="2" t="n">
+      <c r="D42" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D42" s="2" t="inlineStr">
+      <c r="E42" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.5km)</t>
         </is>
@@ -1308,13 +1519,18 @@
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
+          <t>https://nassausuite.com/</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="inlineStr">
+        <is>
           <t>IQWebBook</t>
         </is>
       </c>
-      <c r="C43" s="2" t="n">
+      <c r="D43" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="D43" s="2" t="inlineStr">
+      <c r="E43" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -1328,13 +1544,18 @@
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
+          <t>https://nationalhotel.com/</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C44" s="2" t="n">
+      <c r="D44" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D44" s="2" t="inlineStr">
+      <c r="E44" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.7km)</t>
         </is>
@@ -1348,13 +1569,18 @@
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
+          <t>https://nikkibeach.com/miami-beach/</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C45" s="2" t="n">
+      <c r="D45" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D45" s="2" t="inlineStr">
+      <c r="E45" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.9km)</t>
         </is>
@@ -1368,13 +1594,18 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
+          <t>https://lowkl.com/property/nine20-apartments-by-lowkl/</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
+        <is>
           <t>Cloudbeds</t>
         </is>
       </c>
-      <c r="C46" s="2" t="n">
+      <c r="D46" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="D46" s="2" t="inlineStr">
+      <c r="E46" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.7km)</t>
         </is>
@@ -1388,13 +1619,18 @@
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
+          <t>https://www.noburestaurants.com/miami/home/?utm_source=google&amp;utm_medium=Yext</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C47" s="2" t="n">
+      <c r="D47" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D47" s="2" t="inlineStr">
+      <c r="E47" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (3.3km)</t>
         </is>
@@ -1408,13 +1644,18 @@
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
+          <t>https://grandwelcomehollywood.guestybookings.com/properties/680ba7a29575860013cf2c54</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
           <t>Guesty</t>
         </is>
       </c>
-      <c r="C48" s="2" t="n">
+      <c r="D48" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D48" s="2" t="inlineStr">
+      <c r="E48" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.5km)</t>
         </is>
@@ -1428,13 +1669,18 @@
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
+          <t>https://www.deco305.com/ocean-drive-beachfront/</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C49" s="2" t="n">
+      <c r="D49" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D49" s="2" t="inlineStr">
+      <c r="E49" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -1448,13 +1694,18 @@
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
+          <t>https://all.deco305.com/listings/233176?googleVR=1&amp;utm_source=google&amp;utm_medium=vacation_rentals</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C50" s="2" t="n">
+      <c r="D50" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D50" s="2" t="inlineStr">
+      <c r="E50" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -1468,13 +1719,18 @@
       </c>
       <c r="B51" s="2" t="inlineStr">
         <is>
+          <t>https://all.deco305.com/listings/233209?googleVR=1&amp;utm_source=google&amp;utm_medium=vacation_rentals</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C51" s="2" t="n">
+      <c r="D51" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D51" s="2" t="inlineStr">
+      <c r="E51" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -1488,13 +1744,18 @@
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
+          <t>https://all.deco305.com/listings/233189?googleVR=1&amp;utm_source=google&amp;utm_medium=vacation_rentals</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C52" s="2" t="n">
+      <c r="D52" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D52" s="2" t="inlineStr">
+      <c r="E52" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -1508,13 +1769,18 @@
       </c>
       <c r="B53" s="2" t="inlineStr">
         <is>
+          <t>https://all.deco305.com/listings/233191?googleVR=1&amp;utm_source=google&amp;utm_medium=vacation_rentals</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C53" s="2" t="n">
+      <c r="D53" s="2" t="n">
         <v>305</v>
       </c>
-      <c r="D53" s="2" t="inlineStr">
+      <c r="E53" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -1528,13 +1794,18 @@
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
+          <t>https://whimstay.com/detail/Ocean-View-and-Direct-Beach-Access-Stunning-Coastal-Oasis/508250?isgoogle=true</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="inlineStr">
+        <is>
           <t>Guesty</t>
         </is>
       </c>
-      <c r="C54" s="2" t="n">
+      <c r="D54" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D54" s="2" t="inlineStr">
+      <c r="E54" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (2.3km)</t>
         </is>
@@ -1548,13 +1819,18 @@
       </c>
       <c r="B55" s="2" t="inlineStr">
         <is>
+          <t>https://oceansidehotelmiamibeach.com/</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C55" s="2" t="n">
+      <c r="D55" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D55" s="2" t="inlineStr">
+      <c r="E55" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (0.6km)</t>
         </is>
@@ -1568,13 +1844,18 @@
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
+          <t>https://www.presidentvillamiami.com/</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
           <t>SiteMinder</t>
         </is>
       </c>
-      <c r="C56" s="2" t="n">
+      <c r="D56" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D56" s="2" t="inlineStr">
+      <c r="E56" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -1588,13 +1869,18 @@
       </c>
       <c r="B57" s="2" t="inlineStr">
         <is>
+          <t>https://mylesrestaurantgroup.com/prime-hotel/</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="inlineStr">
+        <is>
           <t>WebRez</t>
         </is>
       </c>
-      <c r="C57" s="2" t="n">
+      <c r="D57" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="D57" s="2" t="inlineStr">
+      <c r="E57" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.8km)</t>
         </is>
@@ -1608,13 +1894,18 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
+          <t>https://www.providentresorts.com/fisher-island-miami</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C58" s="2" t="n">
+      <c r="D58" s="2" t="n">
         <v>170</v>
       </c>
-      <c r="D58" s="2" t="inlineStr">
+      <c r="E58" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (3.2km)</t>
         </is>
@@ -1628,13 +1919,18 @@
       </c>
       <c r="B59" s="2" t="inlineStr">
         <is>
+          <t>https://www.redsouthbeachhotel.com/</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="inlineStr">
+        <is>
           <t>Windsurfer CRS</t>
         </is>
       </c>
-      <c r="C59" s="2" t="n">
+      <c r="D59" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D59" s="2" t="inlineStr">
+      <c r="E59" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (2.3km)</t>
         </is>
@@ -1648,13 +1944,18 @@
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
+          <t>https://lowkl.com/property/rock-apartments-by-lowkl/</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
           <t>Cloudbeds</t>
         </is>
       </c>
-      <c r="C60" s="2" t="n">
+      <c r="D60" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="D60" s="2" t="inlineStr">
+      <c r="E60" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -1668,13 +1969,18 @@
       </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
+          <t>https://www.southbeachluxuryoceanviewhotel.com/</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="inlineStr">
+        <is>
           <t>Cloudbeds</t>
         </is>
       </c>
-      <c r="C61" s="2" t="n">
+      <c r="D61" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D61" s="2" t="inlineStr">
+      <c r="E61" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -1688,13 +1994,18 @@
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
+          <t>https://www.sagamoresouthbeach.com/</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C62" s="2" t="n">
+      <c r="D62" s="2" t="n">
         <v>101</v>
       </c>
-      <c r="D62" s="2" t="inlineStr">
+      <c r="E62" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.6km)</t>
         </is>
@@ -1708,13 +2019,18 @@
       </c>
       <c r="B63" s="2" t="inlineStr">
         <is>
+          <t>https://lowkl.com/property/samantha-apartments-by-lowkl/</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="inlineStr">
+        <is>
           <t>Cloudbeds</t>
         </is>
       </c>
-      <c r="C63" s="2" t="n">
+      <c r="D63" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D63" s="2" t="inlineStr">
+      <c r="E63" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (2.3km)</t>
         </is>
@@ -1728,13 +2044,18 @@
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
+          <t>https://www.sohohouse.com/houses/soho-beach-house?utm_source=google&amp;utm_medium=organic&amp;utm_campaign=googlemybusiness</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C64" s="2" t="n">
+      <c r="D64" s="2" t="n">
         <v>49</v>
       </c>
-      <c r="D64" s="2" t="inlineStr">
+      <c r="E64" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (3.4km)</t>
         </is>
@@ -1748,13 +2069,18 @@
       </c>
       <c r="B65" s="2" t="inlineStr">
         <is>
+          <t>http://www.southbeachhotel.com/</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C65" s="2" t="n">
+      <c r="D65" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D65" s="2" t="inlineStr">
+      <c r="E65" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.2km)</t>
         </is>
@@ -1768,13 +2094,18 @@
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
+          <t>https://alexanderhotel.holidayfuture.com/listings/190221?googleVR=1&amp;utm_source=google&amp;utm_medium=vacation_rentals</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C66" s="2" t="n">
+      <c r="D66" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D66" s="2" t="inlineStr">
+      <c r="E66" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (2.1km)</t>
         </is>
@@ -1788,13 +2119,18 @@
       </c>
       <c r="B67" s="2" t="inlineStr">
         <is>
+          <t>http://www.starlitehotel.com/</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="inlineStr">
+        <is>
           <t>Cloudbeds</t>
         </is>
       </c>
-      <c r="C67" s="2" t="n">
+      <c r="D67" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D67" s="2" t="inlineStr">
+      <c r="E67" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.9km)</t>
         </is>
@@ -1808,13 +2144,18 @@
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
+          <t>https://www.strandoceandrivesuites.com/</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
           <t>SiteMinder</t>
         </is>
       </c>
-      <c r="C68" s="2" t="n">
+      <c r="D68" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D68" s="2" t="inlineStr">
+      <c r="E68" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.5km)</t>
         </is>
@@ -1828,13 +2169,18 @@
       </c>
       <c r="B69" s="2" t="inlineStr">
         <is>
+          <t>https://www.alexanderhotel.com/</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C69" s="2" t="n">
+      <c r="D69" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D69" s="2" t="inlineStr">
+      <c r="E69" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (2.1km)</t>
         </is>
@@ -1848,13 +2194,18 @@
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
+          <t>https://www.thebetsyhotel.com/?utm_source=google-gbp&amp;utm_medium=organic&amp;utm_campaign=gbp</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="inlineStr">
+        <is>
           <t>Triptease</t>
         </is>
       </c>
-      <c r="C70" s="2" t="n">
+      <c r="D70" s="2" t="n">
         <v>1564</v>
       </c>
-      <c r="D70" s="2" t="inlineStr">
+      <c r="E70" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.1km)</t>
         </is>
@@ -1868,13 +2219,18 @@
       </c>
       <c r="B71" s="2" t="inlineStr">
         <is>
+          <t>https://www.gatessouthbeach.com/</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="inlineStr">
+        <is>
           <t>Hilton</t>
         </is>
       </c>
-      <c r="C71" s="2" t="n">
+      <c r="D71" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="D71" s="2" t="inlineStr">
+      <c r="E71" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.5km)</t>
         </is>
@@ -1888,13 +2244,18 @@
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
+          <t>https://themarchhotel.com/?utm_source=google&amp;utm_medium=Local+SEO&amp;utm_campaign=Google+Business+Profile</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C72" s="2" t="n">
+      <c r="D72" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="D72" s="2" t="inlineStr">
+      <c r="E72" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.4km)</t>
         </is>
@@ -1908,13 +2269,18 @@
       </c>
       <c r="B73" s="2" t="inlineStr">
         <is>
+          <t>https://www.thepalmshotel.com/?utm_source=google&amp;utm_medium=organic&amp;utm_campaign=business-listing</t>
+        </is>
+      </c>
+      <c r="C73" s="2" t="inlineStr">
+        <is>
           <t>Triptease</t>
         </is>
       </c>
-      <c r="C73" s="2" t="n">
+      <c r="D73" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D73" s="2" t="inlineStr">
+      <c r="E73" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (2.3km)</t>
         </is>
@@ -1928,13 +2294,18 @@
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
+          <t>http://www.theplymouth.com/</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C74" s="2" t="n">
+      <c r="D74" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D74" s="2" t="inlineStr">
+      <c r="E74" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.2km)</t>
         </is>
@@ -1948,13 +2319,18 @@
       </c>
       <c r="B75" s="2" t="inlineStr">
         <is>
+          <t>https://www.thesetaihotel.com/?utm_source=local&amp;utm_campaign=GMB&amp;utm_medium=organic</t>
+        </is>
+      </c>
+      <c r="C75" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C75" s="2" t="n">
+      <c r="D75" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D75" s="2" t="inlineStr">
+      <c r="E75" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.1km)</t>
         </is>
@@ -1968,13 +2344,18 @@
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
+          <t>https://theshepleyhotel.com/</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="inlineStr">
+        <is>
           <t>IQWebBook</t>
         </is>
       </c>
-      <c r="C76" s="2" t="n">
+      <c r="D76" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="D76" s="2" t="inlineStr">
+      <c r="E76" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.2km)</t>
         </is>
@@ -1988,13 +2369,18 @@
       </c>
       <c r="B77" s="2" t="inlineStr">
         <is>
+          <t>https://www.thewestgem.com/</t>
+        </is>
+      </c>
+      <c r="C77" s="2" t="inlineStr">
+        <is>
           <t>Cloudbeds</t>
         </is>
       </c>
-      <c r="C77" s="2" t="n">
+      <c r="D77" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D77" s="2" t="inlineStr">
+      <c r="E77" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.2km)</t>
         </is>
@@ -2008,13 +2394,18 @@
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
+          <t>https://stayviax.com/hotel/72229962</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="inlineStr">
+        <is>
           <t>proprietary_or_same_domain</t>
         </is>
       </c>
-      <c r="C78" s="2" t="n">
+      <c r="D78" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D78" s="2" t="inlineStr">
+      <c r="E78" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (1.1km)</t>
         </is>
@@ -2028,13 +2419,18 @@
       </c>
       <c r="B79" s="2" t="inlineStr">
         <is>
+          <t>https://www.viajerohostels.com/en/destinations-eeuu/miami-south-beach/</t>
+        </is>
+      </c>
+      <c r="C79" s="2" t="inlineStr">
+        <is>
           <t>BookAssist</t>
         </is>
       </c>
-      <c r="C79" s="2" t="n">
+      <c r="D79" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D79" s="2" t="inlineStr">
+      <c r="E79" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.4km)</t>
         </is>
@@ -2048,13 +2444,18 @@
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
+          <t>https://dreamvillas.holidayfuture.com/listings/178346?googleVR=1&amp;utm_source=google&amp;utm_medium=vacation_rentals</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
           <t>Hostaway</t>
         </is>
       </c>
-      <c r="C80" s="2" t="n">
+      <c r="D80" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D80" s="2" t="inlineStr">
+      <c r="E80" s="2" t="inlineStr">
         <is>
           <t>Nearest: Sherry Frontenac Hotel (2.2km)</t>
         </is>
@@ -2068,13 +2469,18 @@
       </c>
       <c r="B81" s="2" t="inlineStr">
         <is>
+          <t>https://www.waldorftowersmiami.com/?utm_medium=organic&amp;utm_source=google&amp;utm_campaign=business-listing</t>
+        </is>
+      </c>
+      <c r="C81" s="2" t="inlineStr">
+        <is>
           <t>SynXis / TravelClick</t>
         </is>
       </c>
-      <c r="C81" s="2" t="n">
+      <c r="D81" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="D81" s="2" t="inlineStr">
+      <c r="E81" s="2" t="inlineStr">
         <is>
           <t>Nearest: Penguin Hotel (0.8km)</t>
         </is>
@@ -2175,7 +2581,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2 (0.6%)</t>
+          <t>82 (23.1%)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">

</xml_diff>